<commit_message>
Extension Installation Green Tech from EU to all the regions
</commit_message>
<xml_diff>
--- a/Act/Act coeff.xlsx
+++ b/Act/Act coeff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/Act/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="519" documentId="8_{09098739-24F5-4595-8E13-EBA926F9E718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAA1712E-06E1-458D-824C-FAF4927C4791}"/>
+  <xr:revisionPtr revIDLastSave="663" documentId="8_{09098739-24F5-4595-8E13-EBA926F9E718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4DB0ABF-5ABA-47E4-8E90-321F9EA0C3B8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" firstSheet="3" activeTab="6" xr2:uid="{F0FFBB4D-3462-4CB2-9D76-7DC3B03F0357}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="15020" firstSheet="4" activeTab="5" xr2:uid="{F0FFBB4D-3462-4CB2-9D76-7DC3B03F0357}"/>
   </bookViews>
   <sheets>
     <sheet name="z_cons(2023)" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="z_rec(2023)" sheetId="5" r:id="rId4"/>
     <sheet name="Share recycling" sheetId="6" r:id="rId5"/>
     <sheet name="Target recycling" sheetId="7" r:id="rId6"/>
-    <sheet name="Allocation matrix" sheetId="8" r:id="rId7"/>
+    <sheet name="Allocation matrix act" sheetId="8" r:id="rId7"/>
+    <sheet name="Allocation matrix base" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="30">
   <si>
     <t>China</t>
   </si>
@@ -9219,7 +9220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66BF563-C855-4D60-9032-AEE603A77B68}">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AI20"/>
     </sheetView>
   </sheetViews>
@@ -14392,8 +14393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A71C650-29E5-471A-BF58-C4804C6594F9}">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14860,7 +14861,7 @@
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>7.22568E-3</v>
@@ -15276,7 +15277,7 @@
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -15692,7 +15693,7 @@
       <c r="A15" s="24"/>
       <c r="B15" s="24"/>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -16108,7 +16109,7 @@
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -16353,8 +16354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED252F2A-3F4A-423D-8A86-74BC4A1FD378}">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18693,4 +18694,1036 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44250E27-31BF-410D-BD33-83DA28D0093D}">
+  <dimension ref="A1:S19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B1" s="22"/>
+      <c r="D1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0.79196416071678566</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0.79196416071678566</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0.79196416071678566</v>
+      </c>
+      <c r="S7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>8.0008399832003335E-2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>8.0008399832003335E-2</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>8.0008399832003335E-2</v>
+      </c>
+      <c r="S11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>7.2028559428811423E-2</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>7.2028559428811423E-2</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>7.2028559428811423E-2</v>
+      </c>
+      <c r="S15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="7">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10">
+        <v>5.5998880022399548E-2</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
+      <c r="M19" s="10">
+        <v>0</v>
+      </c>
+      <c r="N19" s="10">
+        <v>5.5998880022399548E-2</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0</v>
+      </c>
+      <c r="P19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>0</v>
+      </c>
+      <c r="R19" s="10">
+        <v>5.5998880022399548E-2</v>
+      </c>
+      <c r="S19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>